<commit_message>
update excel for 51visa
</commit_message>
<xml_diff>
--- a/public/group_jcic.xlsx
+++ b/public/group_jcic.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>日本旅行社名</t>
   </si>
@@ -146,12 +146,6 @@
 7-18-5 ソフイアビル 212号室
 担当者：東木慶新
 電話：03-3470-6851</t>
-  </si>
-  <si>
-    <t>http://123.56.136.55/code</t>
-  </si>
-  <si>
-    <t>※编号请查询</t>
   </si>
   <si>
     <t>性别</t>
@@ -572,7 +566,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -616,7 +610,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -665,7 +659,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -709,7 +703,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1022,7 +1016,7 @@
   <dimension ref="A1:G986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1109,7 +1103,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1151,12 +1145,8 @@
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>39</v>
-      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1222,7 +1212,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1232,10 +1222,10 @@
     <row r="19" spans="1:7" ht="14.25" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1245,10 +1235,10 @@
     <row r="20" spans="1:7" ht="14.25" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1258,10 +1248,10 @@
     <row r="21" spans="1:7" ht="14.25" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1271,10 +1261,10 @@
     <row r="22" spans="1:7" ht="14.25" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1284,10 +1274,10 @@
     <row r="23" spans="1:7" ht="28.25" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1297,10 +1287,10 @@
     <row r="24" spans="1:7" ht="14.25" customHeight="1">
       <c r="A24" s="6"/>
       <c r="B24" s="30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -8041,9 +8031,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="22"/>
-  <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -14671,7 +14658,7 @@
         <v>43079</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>35</v>
@@ -19772,7 +19759,6 @@
       <c r="C1003" s="7"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="6">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A3:C3"/>

</xml_diff>